<commit_message>
Changed credentials to CSV format, other fixes
</commit_message>
<xml_diff>
--- a/files/cargahstemplate.xlsx
+++ b/files/cargahstemplate.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t xml:space="preserve">Date</t>
+    <t xml:space="preserve">Date (DD/MM/YYYY)</t>
   </si>
   <si>
     <t xml:space="preserve">Project</t>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t xml:space="preserve">Hello world</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hello world 2</t>
   </si>
 </sst>
 </file>
@@ -172,12 +169,13 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.59"/>
   </cols>
   <sheetData>
@@ -215,7 +213,7 @@
         <v>152</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -224,46 +222,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>44628</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>152</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>44629</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>235</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>